<commit_message>
consider other factors of VMT
</commit_message>
<xml_diff>
--- a/CAORAN.xlsx
+++ b/CAORAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelt/datahere/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34150A1C-9039-46F4-B913-A08ECCEBED01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0E0848-83E4-C74C-B7E2-EAAB33D3A56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="1590" windowWidth="21600" windowHeight="11490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2080" yWindow="1600" windowWidth="21600" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRED Graph" sheetId="1" r:id="rId1"/>
@@ -141,34 +141,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,868 +466,826 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="2" customWidth="1"/>
-    <col min="2" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="20" customWidth="1"/>
-    <col min="9" max="256" width="20.7109375" customWidth="1"/>
+    <col min="1" max="256" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2">
         <v>1970</v>
       </c>
       <c r="B2" s="1">
         <v>1421.2329999999999</v>
       </c>
-      <c r="H2"/>
-      <c r="I2" s="20"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
         <v>1971</v>
       </c>
       <c r="B3" s="1">
         <v>1484.2</v>
       </c>
-      <c r="H3"/>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4">
         <v>1972</v>
       </c>
       <c r="B4" s="1">
         <v>1536.8</v>
       </c>
-      <c r="H4"/>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5">
         <v>1973</v>
       </c>
       <c r="B5" s="1">
         <v>1607.1</v>
       </c>
-      <c r="H5"/>
-      <c r="I5" s="20"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6">
         <v>1974</v>
       </c>
       <c r="B6" s="1">
         <v>1669.1</v>
       </c>
-      <c r="H6"/>
-      <c r="I6" s="20"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7">
         <v>1975</v>
       </c>
       <c r="B7" s="1">
         <v>1725.7</v>
       </c>
-      <c r="H7"/>
-      <c r="I7" s="20"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>1976</v>
       </c>
       <c r="B8" s="1">
         <v>1772.7</v>
       </c>
-      <c r="H8"/>
-      <c r="I8" s="20"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9">
         <v>1977</v>
       </c>
       <c r="B9" s="1">
         <v>1812.1</v>
       </c>
-      <c r="H9"/>
-      <c r="I9" s="20"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10">
         <v>1978</v>
       </c>
       <c r="B10" s="1">
         <v>1853.1</v>
       </c>
-      <c r="H10"/>
-      <c r="I10" s="20"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11">
         <v>1979</v>
       </c>
       <c r="B11" s="1">
         <v>1892</v>
       </c>
-      <c r="H11"/>
-      <c r="I11" s="20"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12">
         <v>1980</v>
       </c>
       <c r="B12" s="1">
         <v>1932.921</v>
       </c>
-      <c r="H12"/>
-      <c r="I12" s="20"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>1981</v>
       </c>
       <c r="B13" s="1">
         <v>2004.806</v>
       </c>
-      <c r="H13"/>
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A14">
         <v>1982</v>
       </c>
       <c r="B14" s="1">
         <v>2045.925</v>
       </c>
-      <c r="H14"/>
-      <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A15">
         <v>1983</v>
       </c>
       <c r="B15" s="1">
         <v>2088.886</v>
       </c>
-      <c r="H15"/>
-      <c r="I15" s="20"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16">
         <v>1984</v>
       </c>
       <c r="B16" s="1">
         <v>2123.3620000000001</v>
       </c>
-      <c r="H16"/>
-      <c r="I16" s="20"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17">
         <v>1985</v>
       </c>
       <c r="B17" s="1">
         <v>2171.9299999999998</v>
       </c>
-      <c r="H17"/>
-      <c r="I17" s="20"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18">
         <v>1986</v>
       </c>
       <c r="B18" s="1">
         <v>2228.895</v>
       </c>
-      <c r="H18"/>
-      <c r="I18" s="20"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19">
         <v>1987</v>
       </c>
       <c r="B19" s="1">
         <v>2281.4859999999999</v>
       </c>
-      <c r="H19"/>
-      <c r="I19" s="20"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20">
         <v>1988</v>
       </c>
       <c r="B20" s="1">
         <v>2333.1010000000001</v>
       </c>
-      <c r="H20"/>
-      <c r="I20" s="20"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A21">
         <v>1989</v>
       </c>
       <c r="B21" s="1">
         <v>2383.92</v>
       </c>
-      <c r="H21"/>
-      <c r="I21" s="21">
+      <c r="I21" s="2">
         <v>39592</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A22">
         <v>1990</v>
       </c>
       <c r="B22" s="1">
         <v>2418.9859999999999</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="3">
         <v>3.5</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="2">
         <v>1305545</v>
       </c>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23">
         <v>1991</v>
       </c>
       <c r="B23" s="1">
         <v>2452.6909999999998</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="3">
         <v>5.3</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="2">
         <v>1251290</v>
       </c>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24">
         <v>1992</v>
       </c>
       <c r="B24" s="1">
         <v>2497.0140000000001</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="3">
         <v>6.7</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="2">
         <v>1240988</v>
       </c>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25">
         <v>1993</v>
       </c>
       <c r="B25" s="1">
         <v>2532.6390000000001</v>
       </c>
-      <c r="G25" s="11">
+      <c r="G25" s="3">
         <v>6.8</v>
       </c>
-      <c r="H25" s="19">
+      <c r="H25" s="2">
         <v>1236273</v>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="2">
         <v>45116</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26">
         <v>1994</v>
       </c>
       <c r="B26" s="1">
         <v>2566.5990000000002</v>
       </c>
-      <c r="G26" s="11">
+      <c r="G26" s="3">
         <v>5.8</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="2">
         <v>1256115</v>
       </c>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A27">
         <v>1995</v>
       </c>
       <c r="B27" s="1">
         <v>2603.6779999999999</v>
       </c>
-      <c r="G27" s="11">
+      <c r="G27" s="3">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="2">
         <v>1255072</v>
       </c>
-      <c r="I27" s="21">
+      <c r="I27" s="2">
         <v>48701</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A28">
         <v>1996</v>
       </c>
       <c r="B28" s="1">
         <v>2643.9960000000001</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G28" s="3">
         <v>4.2</v>
       </c>
-      <c r="H28" s="19">
+      <c r="H28" s="2">
         <v>1275059</v>
       </c>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29">
         <v>1997</v>
       </c>
       <c r="B29" s="1">
         <v>2709.277</v>
       </c>
-      <c r="G29" s="11">
+      <c r="G29" s="3">
         <v>3.3</v>
       </c>
-      <c r="H29" s="19">
+      <c r="H29" s="2">
         <v>1328578</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I29" s="2">
         <v>49583</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A30">
         <v>1998</v>
       </c>
       <c r="B30" s="1">
         <v>2773.1869999999999</v>
       </c>
-      <c r="G30" s="11">
+      <c r="G30" s="3">
         <v>2.9</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="2">
         <v>1386214</v>
       </c>
-      <c r="I30" s="21">
+      <c r="I30" s="2">
         <v>50986</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A31">
         <v>1999</v>
       </c>
       <c r="B31" s="1">
         <v>2815.933</v>
       </c>
-      <c r="G31" s="11">
+      <c r="G31" s="3">
         <v>2.7</v>
       </c>
-      <c r="H31" s="19">
+      <c r="H31" s="2">
         <v>1423834</v>
       </c>
-      <c r="I31" s="21">
+      <c r="I31" s="2">
         <v>52129</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A32">
         <v>2000</v>
       </c>
       <c r="B32" s="1">
         <v>2856.241</v>
       </c>
-      <c r="G32" s="11">
+      <c r="G32" s="3">
         <v>3.5</v>
       </c>
-      <c r="H32" s="19">
+      <c r="H32" s="2">
         <v>1428975</v>
       </c>
-      <c r="I32" s="21">
+      <c r="I32" s="2">
         <v>55654</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A33">
         <v>2001</v>
       </c>
       <c r="B33" s="1">
         <v>2890.6840000000002</v>
       </c>
-      <c r="G33" s="11">
+      <c r="G33" s="3">
         <v>4</v>
       </c>
-      <c r="H33" s="19">
+      <c r="H33" s="2">
         <v>1449080</v>
       </c>
-      <c r="I33" s="21">
+      <c r="I33" s="2">
         <v>55994</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A34">
         <v>2002</v>
       </c>
       <c r="B34" s="1">
         <v>2917.1619999999998</v>
       </c>
-      <c r="G34" s="11">
+      <c r="G34" s="3">
         <v>5</v>
       </c>
-      <c r="H34" s="19">
+      <c r="H34" s="2">
         <v>1447724</v>
       </c>
-      <c r="I34" s="21">
+      <c r="I34" s="2">
         <v>55992</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A35">
         <v>2003</v>
       </c>
       <c r="B35" s="1">
         <v>2941.5729999999999</v>
       </c>
-      <c r="G35" s="11">
+      <c r="G35" s="3">
         <v>4.8</v>
       </c>
-      <c r="H35" s="19">
+      <c r="H35" s="2">
         <v>1470827</v>
       </c>
-      <c r="I35" s="21">
+      <c r="I35" s="2">
         <v>55909</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A36">
         <v>2004</v>
       </c>
       <c r="B36" s="1">
         <v>2956.4609999999998</v>
       </c>
-      <c r="G36" s="11">
+      <c r="G36" s="3">
         <v>4.2</v>
       </c>
-      <c r="H36" s="19">
+      <c r="H36" s="2">
         <v>1502003</v>
       </c>
-      <c r="I36" s="21">
+      <c r="I36" s="2">
         <v>58605</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A37">
         <v>2005</v>
       </c>
       <c r="B37" s="1">
         <v>2957.404</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G37" s="3">
         <v>3.7</v>
       </c>
-      <c r="H37" s="19">
+      <c r="H37" s="2">
         <v>1527005</v>
       </c>
-      <c r="I37" s="21">
+      <c r="I37" s="2">
         <v>65823</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A38">
         <v>2006</v>
       </c>
       <c r="B38" s="1">
         <v>2952.61</v>
       </c>
-      <c r="G38" s="11">
+      <c r="G38" s="3">
         <v>3.4</v>
       </c>
-      <c r="H38" s="19">
+      <c r="H38" s="2">
         <v>1546035</v>
       </c>
-      <c r="I38" s="21">
+      <c r="I38" s="2">
         <v>70109</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A39">
         <v>2007</v>
       </c>
       <c r="B39" s="1">
         <v>2957.3069999999998</v>
       </c>
-      <c r="G39" s="11">
+      <c r="G39" s="3">
         <v>3.8</v>
       </c>
-      <c r="H39" s="19">
+      <c r="H39" s="2">
         <v>1546709</v>
       </c>
-      <c r="I39" s="21">
+      <c r="I39" s="2">
         <v>73107</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A40">
         <v>2008</v>
       </c>
       <c r="B40" s="1">
         <v>2988.5410000000002</v>
       </c>
-      <c r="G40" s="11">
+      <c r="G40" s="3">
         <v>5.3</v>
       </c>
-      <c r="H40" s="19">
+      <c r="H40" s="2">
         <v>1530120</v>
       </c>
-      <c r="I40" s="21">
+      <c r="I40" s="2">
         <v>74862</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A41">
         <v>2009</v>
       </c>
       <c r="B41" s="1">
         <v>3023.2649999999999</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="3">
         <v>9</v>
       </c>
-      <c r="H41" s="19">
+      <c r="H41" s="2">
         <v>1451508</v>
       </c>
-      <c r="I41" s="21">
+      <c r="I41" s="2">
         <v>71735</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42">
         <v>2010</v>
       </c>
       <c r="B42" s="1">
         <v>3016.3760000000002</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="3">
         <v>10</v>
       </c>
-      <c r="H42" s="19">
+      <c r="H42" s="2">
         <v>1383916</v>
       </c>
-      <c r="I42" s="21">
+      <c r="I42" s="2">
         <v>70727</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43">
         <v>2011</v>
       </c>
       <c r="B43" s="1">
         <v>3050.1990000000001</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="3">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H43" s="19">
+      <c r="H43" s="2">
         <v>1400874</v>
       </c>
-      <c r="I43" s="21">
+      <c r="I43" s="2">
         <v>72046</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44">
         <v>2012</v>
       </c>
       <c r="B44" s="1">
         <v>3078.71</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="3">
         <v>8</v>
       </c>
-      <c r="H44" s="19">
+      <c r="H44" s="2">
         <v>1433508</v>
       </c>
-      <c r="I44" s="21">
+      <c r="I44" s="2">
         <v>71866</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45">
         <v>2013</v>
       </c>
       <c r="B45" s="1">
         <v>3105.2620000000002</v>
       </c>
-      <c r="G45" s="11">
+      <c r="G45" s="3">
         <v>6.7</v>
       </c>
-      <c r="H45" s="19">
+      <c r="H45" s="2">
         <v>1455311</v>
       </c>
-      <c r="I45" s="21">
+      <c r="I45" s="2">
         <v>73827</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46">
         <v>2014</v>
       </c>
       <c r="B46" s="1">
         <v>3126.5230000000001</v>
       </c>
-      <c r="G46" s="11">
+      <c r="G46" s="3">
         <v>5.6</v>
       </c>
-      <c r="H46" s="19">
+      <c r="H46" s="2">
         <v>1478476</v>
       </c>
-      <c r="I46" s="21">
+      <c r="I46" s="2">
         <v>76061</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47">
         <v>2015</v>
       </c>
       <c r="B47" s="1">
         <v>3148.9520000000002</v>
       </c>
-      <c r="G47" s="11">
+      <c r="G47" s="3">
         <v>4.5</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47" s="2">
         <v>1513060</v>
       </c>
-      <c r="I47" s="21">
+      <c r="I47" s="2">
         <v>78002</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48">
         <v>2016</v>
       </c>
       <c r="B48" s="1">
         <v>3164.277</v>
       </c>
-      <c r="G48" s="11">
+      <c r="G48" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H48" s="19">
+      <c r="H48" s="2">
         <v>1532725</v>
       </c>
-      <c r="I48" s="21">
+      <c r="I48" s="2">
         <v>81642</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A49">
         <v>2017</v>
       </c>
       <c r="B49" s="1">
         <v>3174.1590000000001</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="2">
         <v>244438165</v>
       </c>
-      <c r="D49" s="17">
+      <c r="D49" s="2">
         <v>244438165</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="3">
         <v>2740550.3</v>
       </c>
-      <c r="F49" s="23">
+      <c r="F49" s="3">
         <v>2740550.3</v>
       </c>
-      <c r="G49" s="11">
+      <c r="G49" s="3">
         <v>3.5</v>
       </c>
-      <c r="H49" s="19">
+      <c r="H49" s="2">
         <v>1549003</v>
       </c>
-      <c r="I49" s="21">
+      <c r="I49" s="2">
         <v>86031</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50">
         <v>2018</v>
       </c>
       <c r="B50" s="1">
         <v>3175.5790000000002</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C50" s="2">
         <v>256068837</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="2">
         <v>251165771</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="3">
         <v>2899530.9</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="3">
         <v>2850970.3</v>
       </c>
-      <c r="G50" s="11">
+      <c r="G50" s="3">
         <v>3</v>
       </c>
-      <c r="H50" s="19">
+      <c r="H50" s="2">
         <v>1568273</v>
       </c>
-      <c r="I50" s="21">
+      <c r="I50" s="2">
         <v>89373</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51">
         <v>2019</v>
       </c>
       <c r="B51" s="1">
         <v>3170.8510000000001</v>
       </c>
-      <c r="C51" s="4">
+      <c r="C51" s="2">
         <v>269080278</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="2">
         <v>257959284</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="3">
         <v>3062158.9</v>
       </c>
-      <c r="F51" s="23">
+      <c r="F51" s="3">
         <v>2962792.1</v>
       </c>
-      <c r="G51" s="11">
+      <c r="G51" s="3">
         <v>2.8</v>
       </c>
-      <c r="H51" s="19">
+      <c r="H51" s="2">
         <v>1571261</v>
       </c>
-      <c r="I51" s="21">
+      <c r="I51" s="2">
         <v>95761</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52">
         <v>2020</v>
       </c>
       <c r="B52" s="1">
         <v>3185.5160000000001</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="2">
         <v>268778347</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="2">
         <v>252505652</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="3">
         <v>3068809.4</v>
       </c>
-      <c r="F52" s="23">
+      <c r="F52" s="3">
         <v>2925146.9</v>
       </c>
-      <c r="G52" s="11">
+      <c r="G52" s="3">
         <v>8.9</v>
       </c>
-      <c r="H52" s="19">
+      <c r="H52" s="2">
         <v>1426971</v>
       </c>
-      <c r="I52" s="21">
+      <c r="I52" s="2">
         <v>98786</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A53">
         <v>2021</v>
       </c>
       <c r="B53" s="1">
         <v>3161.0050000000001</v>
       </c>
-      <c r="C53" s="4">
+      <c r="C53" s="2">
         <v>294339604</v>
       </c>
-      <c r="D53" s="17">
+      <c r="D53" s="2">
         <v>268128135</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="3">
         <v>3416939.4</v>
       </c>
-      <c r="F53" s="23">
+      <c r="F53" s="3">
         <v>3146185.3</v>
       </c>
-      <c r="G53" s="11">
+      <c r="G53" s="3">
         <v>6</v>
       </c>
-      <c r="H53" s="19">
+      <c r="H53" s="2">
         <v>1467342</v>
       </c>
-      <c r="I53" s="21">
+      <c r="I53" s="2">
         <v>100210</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A54">
         <v>2022</v>
       </c>
       <c r="B54" s="1">
         <v>3151.1840000000002</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="2">
         <v>314177082</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="2">
         <v>270440831</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="3">
         <v>3641643.4</v>
       </c>
-      <c r="F54" s="23">
+      <c r="F54" s="3">
         <v>3167460.8</v>
       </c>
-      <c r="G54" s="11">
+      <c r="G54" s="3">
         <v>3.2</v>
       </c>
-      <c r="H54" s="19">
+      <c r="H54" s="2">
         <v>1540561</v>
       </c>
-      <c r="I54" s="21">
+      <c r="I54" s="2">
         <v>106047</v>
       </c>
     </row>
@@ -1367,73 +1305,73 @@
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1451,34 +1389,34 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>5</v>
       </c>

</xml_diff>